<commit_message>
CyTOF with corrected standard error
</commit_message>
<xml_diff>
--- a/experimental_data.xlsx
+++ b/experimental_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies Lineage Marker" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="83">
   <si>
     <t xml:space="preserve">Sample</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t xml:space="preserve">AnAr_20171026_11_normalized.fcs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">repeat 2</t>
   </si>
   <si>
     <t xml:space="preserve">AnAr_20171026_12_normalized.fcs</t>
@@ -281,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -303,6 +300,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -479,13 +482,23 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{3D332D16-CA17-44D9-B6B2-4A632D19AA70}">
-  <header guid="{70060138-AF25-4A4E-9F3D-CF723B8544CF}" dateTime="2017-11-24T10:56:00.000000000Z" userName="Angela Ariza" r:id="rId1" minRId="1" maxRId="24" maxSheetId="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{9809D042-C3FF-4C24-A45C-C1E6CFCF80CE}">
+  <header guid="{28709162-AB32-4993-8D09-C5D69EB50B8C}" dateTime="2017-11-24T10:56:00.000000000Z" userName="Angela Ariza" r:id="rId1" minRId="1" maxRId="24" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{3D332D16-CA17-44D9-B6B2-4A632D19AA70}" dateTime="2017-11-24T11:26:00.000000000Z" userName="Angela Ariza" r:id="rId2" minRId="25" maxRId="25" maxSheetId="2">
+  <header guid="{874C9ED5-2BF6-48E3-9CCC-F4EED5A6062A}" dateTime="2017-11-24T11:26:00.000000000Z" userName="Angela Ariza" r:id="rId2" minRId="25" maxRId="25" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3327C981-F218-47BC-833B-F2067560C97E}" dateTime="2018-05-28T14:36:00.000000000Z" userName=" " r:id="rId3" minRId="26" maxRId="27" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9809D042-C3FF-4C24-A45C-C1E6CFCF80CE}" dateTime="2018-05-30T13:09:00.000000000Z" userName=" " r:id="rId4" minRId="28" maxRId="30" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -500,8 +513,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -519,8 +531,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -538,8 +549,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -552,8 +562,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -568,8 +577,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -587,8 +595,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -606,8 +613,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -620,8 +626,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -636,8 +641,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -655,8 +659,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -674,8 +677,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -693,8 +695,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -712,8 +713,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -726,8 +726,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -742,8 +741,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -761,8 +759,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -780,8 +777,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -794,8 +790,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -810,8 +805,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -829,8 +823,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -848,8 +841,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -867,8 +859,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -886,8 +877,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -900,8 +890,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -916,8 +905,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -935,8 +923,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -954,8 +941,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -968,8 +954,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -984,8 +969,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -1003,8 +987,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -1027,8 +1010,7 @@
       <is>
         <r>
           <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -1036,6 +1018,84 @@
           <t xml:space="preserve">Cell populations:</t>
         </r>
       </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="26" ua="false" sId="1">
+    <nc r="D3" t="n">
+      <f>SUM(E4:J4)</f>
+    </nc>
+  </rcc>
+  <rcc rId="27" ua="false" sId="1">
+    <oc r="D3" t="n">
+      <f>SUM(E4:J4)</f>
+    </oc>
+    <nc r="D3"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="28" ua="false" sId="1">
+    <oc r="B22" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">repeat 2</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B22" t="n">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="29" ua="false" sId="1">
+    <oc r="B23" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">repeat 2</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B23" t="n">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="30" ua="false" sId="1">
+    <oc r="B24" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">repeat 2</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B24" t="n">
+      <v>2</v>
     </nc>
   </rcc>
 </revisions>
@@ -1052,22 +1112,22 @@
   </sheetPr>
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3906976744186"/>
-    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="11.5860465116279"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.0744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="12" style="0" width="11.5860465116279"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.4651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5860465116279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.0651162790698"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9255813953488"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.893023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9767441860465"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.8976744186047"/>
+    <col collapsed="false" hidden="false" max="16" min="12" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="12.0604651162791"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,7 +1365,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3519,8 +3579,8 @@
       <c r="A22" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>69</v>
+      <c r="B22" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>58</v>
@@ -3639,10 +3699,10 @@
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="6" t="s">
         <v>69</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>58</v>
@@ -3761,10 +3821,10 @@
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>58</v>
@@ -3921,7 +3981,7 @@
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>3</v>
@@ -4043,7 +4103,7 @@
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>3</v>
@@ -4165,7 +4225,7 @@
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>3</v>
@@ -4287,7 +4347,7 @@
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>3</v>
@@ -4409,7 +4469,7 @@
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>3</v>
@@ -4531,7 +4591,7 @@
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>3</v>
@@ -4653,7 +4713,7 @@
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -4775,7 +4835,7 @@
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>3</v>
@@ -4897,7 +4957,7 @@
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>3</v>
@@ -5019,7 +5079,7 @@
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>3</v>
@@ -5141,7 +5201,7 @@
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>46.1</v>
@@ -5254,7 +5314,7 @@
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>6.35</v>

</xml_diff>